<commit_message>
updates to application and fixed bug in trebuchet.py
</commit_message>
<xml_diff>
--- a/test/data/sample_results.xlsx
+++ b/test/data/sample_results.xlsx
@@ -476,13 +476,13 @@
         <v>5</v>
       </c>
       <c r="D2" t="n">
-        <v>47.759</v>
+        <v>11.429</v>
       </c>
       <c r="E2" t="n">
-        <v>18.326</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>3.15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -496,13 +496,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>56.549</v>
+        <v>11.424</v>
       </c>
       <c r="E3" t="n">
-        <v>18.609</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>3.25</v>
+        <v>10.017</v>
       </c>
     </row>
     <row r="4">
@@ -516,13 +516,13 @@
         <v>15</v>
       </c>
       <c r="D4" t="n">
-        <v>44.112</v>
+        <v>11.36</v>
       </c>
       <c r="E4" t="n">
-        <v>18.718</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>3.6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
@@ -536,13 +536,13 @@
         <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>30.447</v>
+        <v>11.418</v>
       </c>
       <c r="E5" t="n">
-        <v>17.904</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>3.867</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -556,13 +556,13 @@
         <v>25</v>
       </c>
       <c r="D6" t="n">
-        <v>18.982</v>
+        <v>2.236</v>
       </c>
       <c r="E6" t="n">
-        <v>16.673</v>
+        <v>5.542</v>
       </c>
       <c r="F6" t="n">
-        <v>4.067</v>
+        <v>4.667</v>
       </c>
     </row>
     <row r="7">
@@ -576,13 +576,13 @@
         <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>10.359</v>
+        <v>32.656</v>
       </c>
       <c r="E7" t="n">
-        <v>15.158</v>
+        <v>29.383</v>
       </c>
       <c r="F7" t="n">
-        <v>4.19</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="8">
@@ -596,13 +596,13 @@
         <v>35</v>
       </c>
       <c r="D8" t="n">
-        <v>5.029</v>
+        <v>52.361</v>
       </c>
       <c r="E8" t="n">
-        <v>13.703</v>
+        <v>54.878</v>
       </c>
       <c r="F8" t="n">
-        <v>4.283</v>
+        <v>4.583</v>
       </c>
     </row>
     <row r="9">
@@ -616,13 +616,13 @@
         <v>40</v>
       </c>
       <c r="D9" t="n">
-        <v>2.236</v>
+        <v>33.347</v>
       </c>
       <c r="E9" t="n">
-        <v>12.482</v>
+        <v>73.331</v>
       </c>
       <c r="F9" t="n">
-        <v>4.381</v>
+        <v>5.02</v>
       </c>
     </row>
     <row r="10">
@@ -639,10 +639,10 @@
         <v>2.236</v>
       </c>
       <c r="E10" t="n">
-        <v>11.483</v>
+        <v>79.49299999999999</v>
       </c>
       <c r="F10" t="n">
-        <v>4.467</v>
+        <v>5.117</v>
       </c>
     </row>
     <row r="11">
@@ -659,10 +659,10 @@
         <v>2.236</v>
       </c>
       <c r="E11" t="n">
-        <v>10.652</v>
+        <v>69.581</v>
       </c>
       <c r="F11" t="n">
-        <v>4.55</v>
+        <v>4.791</v>
       </c>
     </row>
     <row r="12">
@@ -679,10 +679,10 @@
         <v>2.236</v>
       </c>
       <c r="E12" t="n">
-        <v>9.951000000000001</v>
+        <v>50.555</v>
       </c>
       <c r="F12" t="n">
-        <v>4.65</v>
+        <v>4.15</v>
       </c>
     </row>
     <row r="13">
@@ -699,10 +699,10 @@
         <v>2.236</v>
       </c>
       <c r="E13" t="n">
-        <v>9.308</v>
+        <v>32.874</v>
       </c>
       <c r="F13" t="n">
-        <v>4.733</v>
+        <v>3.433</v>
       </c>
     </row>
     <row r="14">
@@ -719,10 +719,10 @@
         <v>2.236</v>
       </c>
       <c r="E14" t="n">
-        <v>8.766</v>
+        <v>19.646</v>
       </c>
       <c r="F14" t="n">
-        <v>4.85</v>
+        <v>2.783</v>
       </c>
     </row>
     <row r="15">
@@ -739,10 +739,10 @@
         <v>2.236</v>
       </c>
       <c r="E15" t="n">
-        <v>8.004</v>
+        <v>10.614</v>
       </c>
       <c r="F15" t="n">
-        <v>4.9</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="16">
@@ -759,10 +759,10 @@
         <v>2.236</v>
       </c>
       <c r="E16" t="n">
-        <v>7.65</v>
+        <v>4.971</v>
       </c>
       <c r="F16" t="n">
-        <v>4.967</v>
+        <v>1.617</v>
       </c>
     </row>
     <row r="17">
@@ -779,10 +779,10 @@
         <v>2.236</v>
       </c>
       <c r="E17" t="n">
-        <v>7.292</v>
+        <v>1.823</v>
       </c>
       <c r="F17" t="n">
-        <v>5.033</v>
+        <v>1.133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>